<commit_message>
Atualização automática de NOVA_PRATA.xlsx
</commit_message>
<xml_diff>
--- a/NOVA_PRATA.xlsx
+++ b/NOVA_PRATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8DE0814-F1BC-46F6-AA03-54A25C249724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3131CA8-F305-4B28-BF93-BC1EADB0FBEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,20 +21,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="5" r:id="rId6"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1113,7 +1100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1173,36 +1160,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1241,14 +1204,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1294,7 +1252,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{EDEA3E74-C09A-4EB2-97EF-F75E5B73BC72}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{41B1C4CD-8B66-4C22-944E-D87CF7A7DC25}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1324,10 +1282,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B86CC56-7260-4B6D-AD2F-508609911D6C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4248D674-733E-401B-ABB3-C388F0C9E935}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1365,7 +1323,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A67DB1EE-80D8-4265-9769-213F3CB057EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03FC8F51-8A66-44F6-82DE-05B1DC033497}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1428,7 +1386,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD5DD755-1431-45FB-AD82-239606EF95F2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CE5BA66-546D-4B22-B13E-18C147D7F963}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1447,7 +1405,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50E396E4-280B-8265-7995-FC7E59958C22}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE49CF64-A2EB-A1CF-8212-C145540D8571}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1496,7 +1454,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F48DAD8-EC06-E7D8-78F9-15D7CA92CB79}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B286DFD4-80D3-5667-FDB3-DF51A48F32E9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1515,7 +1473,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B3EB381-44D9-C628-0B34-CC61644373D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A73849E-45BA-AF8D-0749-0604F279DFB7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1546,7 +1504,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B994C04D-DA7F-4E80-F71E-B6041C94EBAE}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFD606A5-72DE-4545-E686-3D331D3FFC78}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1577,7 +1535,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E076A734-F548-E375-023B-7BFD45BD752D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D389AD9E-06DA-E51D-0E62-9305554DCE01}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1620,7 +1578,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B6D0D86-0CA9-4B85-ADE0-F278886BCB39}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2218610-B2AB-469C-8241-9B225FE71247}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1658,7 +1616,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{621063FC-B224-4317-8697-019C7B15ECB0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21E2E4F7-D8B0-420E-BAD1-9BC09A7CFCA8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1701,7 +1659,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C4DB30E-9E78-4961-BB3D-A46961198E5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A201B95-1135-479F-8556-AE4B2BBD6BC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2014,7 +1972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3FAA2C-D51F-4174-BF0C-9391C8D9D7EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296B8C2C-4EA7-4F86-8C3E-E0511ABD9A93}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2026,98 +1984,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="37"/>
-    <col min="6" max="6" width="2" style="37" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="37"/>
+    <col min="1" max="5" width="12.5703125" style="34"/>
+    <col min="6" max="6" width="2" style="34" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="34" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="36"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="36"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="36"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="36"/>
+      <c r="F4" s="33"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="36"/>
+      <c r="F5" s="33"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="36"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="36"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="36"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="36"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="36"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="36"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="36"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="36"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="36"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="36"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="36"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="36"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="36"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="36"/>
+      <c r="F19" s="33"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="36"/>
+      <c r="F20" s="33"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="36"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="36"/>
+      <c r="F22" s="33"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="36"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="36"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="36"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="36"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="36"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="36"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="36"/>
+      <c r="F29" s="33"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5635,19 +5593,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>288</v>
       </c>
     </row>
@@ -5670,46 +5628,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>291</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>292</v>
       </c>
     </row>
@@ -5734,54 +5692,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="21" t="s">
         <v>296</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>297</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="21" t="s">
         <v>298</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="G1" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>304</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="20" t="s">
         <v>307</v>
       </c>
-      <c r="N1" s="23" t="s">
+      <c r="N1" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="O1" s="23" t="s">
+      <c r="O1" s="20" t="s">
         <v>309</v>
       </c>
     </row>
@@ -5792,43 +5751,43 @@
       <c r="B2" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="23">
         <v>45108</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="24">
         <v>3489</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>311</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="25">
         <v>8924</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="25">
         <v>1345</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="H2" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="26" t="s">
         <v>312</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="K2" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="L2" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="26" t="s">
         <v>312</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="O2" s="30" t="s">
+      <c r="O2" s="27" t="s">
         <v>314</v>
       </c>
     </row>
@@ -5859,25 +5818,24 @@
       <c r="B1" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>316</v>
       </c>
-      <c r="E1" s="32">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="29">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="32">
         <v>81</v>
       </c>
-      <c r="F1" s="33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>317</v>
-      </c>
-      <c r="B2" s="35">
-        <v>81</v>
-      </c>
-      <c r="C2" s="33">
+      <c r="C2" s="30">
         <v>5.3564343340827929E-3</v>
       </c>
     </row>

</xml_diff>